<commit_message>
Updated version of menu and PS table (2023_v1_0_1)
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2023_v1_0_1/PrescaleTable/L1Menu_Collisions2023_v1_0_1.xlsx
+++ b/development/L1Menu_Collisions2023_v1_0_1/PrescaleTable/L1Menu_Collisions2023_v1_0_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DAF69A-D141-3B41-8872-9DAD0FA0C7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E9FE8-251F-D047-AB9C-F2D411E75AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="-18220" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4560" yWindow="-17680" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1Menu_Collisions2023_v1_0_0" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="440">
   <si>
     <t>Emergency</t>
   </si>
@@ -1354,15 +1354,6 @@
   <si>
     <t>OnlyMuons</t>
   </si>
-  <si>
-    <t>L1_DoubleMu0_Upt6_IP_Min1_Upt4_IP_Min1</t>
-  </si>
-  <si>
-    <t>L1_DoubleMu0_Upt6_IP_Min1_Upt6</t>
-  </si>
-  <si>
-    <t>L1_DoubleMu0_Upt6_IP_Min1_Upt6_IP_Min1</t>
-  </si>
 </sst>
 </file>
 
@@ -1487,31 +1478,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1798,13 +1765,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1013"/>
+  <dimension ref="A1:AD1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M382" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N412" sqref="N412"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6862,67 +6829,67 @@
         <v>0</v>
       </c>
       <c r="D69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -6936,67 +6903,67 @@
         <v>0</v>
       </c>
       <c r="D70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -7602,67 +7569,67 @@
         <v>0</v>
       </c>
       <c r="D79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -16713,7 +16680,7 @@
         <v>2</v>
       </c>
       <c r="G202" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H202" s="5">
         <v>1</v>
@@ -20700,7 +20667,7 @@
         <v>0</v>
       </c>
       <c r="D256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E256" s="5">
         <v>0</v>
@@ -20712,55 +20679,55 @@
         <v>0</v>
       </c>
       <c r="H256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -24548,7 +24515,7 @@
         <v>0</v>
       </c>
       <c r="D308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E308" s="5">
         <v>0</v>
@@ -24557,58 +24524,58 @@
         <v>0</v>
       </c>
       <c r="G308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29802,7 +29769,7 @@
         <v>17881</v>
       </c>
       <c r="D379" s="9">
-        <v>20219</v>
+        <v>18013</v>
       </c>
       <c r="E379" s="9">
         <v>18013</v>
@@ -29817,7 +29784,7 @@
         <v>18013</v>
       </c>
       <c r="I379" s="9">
-        <v>20219</v>
+        <v>18013</v>
       </c>
       <c r="J379" s="9">
         <v>18013</v>
@@ -29876,7 +29843,7 @@
         <v>0</v>
       </c>
       <c r="D380" s="9">
-        <v>13781</v>
+        <v>54039</v>
       </c>
       <c r="E380" s="9">
         <v>54039</v>
@@ -29891,7 +29858,7 @@
         <v>54039</v>
       </c>
       <c r="I380" s="9">
-        <v>13781</v>
+        <v>54039</v>
       </c>
       <c r="J380" s="9">
         <v>54039</v>
@@ -32678,226 +32645,76 @@
       </c>
     </row>
     <row r="418" spans="1:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="A418" s="4">
-        <v>508</v>
-      </c>
-      <c r="B418" t="s">
-        <v>440</v>
-      </c>
-      <c r="C418" s="5">
-        <v>0</v>
-      </c>
-      <c r="D418" s="5">
-        <v>0</v>
-      </c>
-      <c r="E418" s="5">
-        <v>0</v>
-      </c>
-      <c r="F418" s="5">
-        <v>0</v>
-      </c>
-      <c r="G418" s="5">
-        <v>0</v>
-      </c>
-      <c r="H418" s="5">
-        <v>0</v>
-      </c>
-      <c r="I418" s="5">
-        <v>0</v>
-      </c>
-      <c r="J418" s="5">
-        <v>0</v>
-      </c>
-      <c r="K418" s="5">
-        <v>0</v>
-      </c>
-      <c r="L418" s="5">
-        <v>0</v>
-      </c>
-      <c r="M418" s="5">
-        <v>0</v>
-      </c>
-      <c r="N418" s="5">
-        <v>0</v>
-      </c>
-      <c r="O418" s="5">
-        <v>0</v>
-      </c>
-      <c r="P418" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q418" s="5">
-        <v>0</v>
-      </c>
-      <c r="R418" s="5">
-        <v>0</v>
-      </c>
-      <c r="S418" s="5">
-        <v>0</v>
-      </c>
-      <c r="T418" s="5">
-        <v>0</v>
-      </c>
-      <c r="U418" s="5">
-        <v>0</v>
-      </c>
-      <c r="V418" s="5">
-        <v>0</v>
-      </c>
-      <c r="W418" s="5">
-        <v>0</v>
-      </c>
-      <c r="X418" s="5">
-        <v>0</v>
-      </c>
+      <c r="C418" s="5"/>
+      <c r="D418" s="5"/>
+      <c r="E418" s="5"/>
+      <c r="F418" s="5"/>
+      <c r="G418" s="5"/>
+      <c r="H418" s="5"/>
+      <c r="I418" s="5"/>
+      <c r="J418" s="5"/>
+      <c r="K418" s="5"/>
+      <c r="L418" s="5"/>
+      <c r="M418" s="5"/>
+      <c r="N418" s="5"/>
+      <c r="O418" s="5"/>
+      <c r="P418" s="5"/>
+      <c r="Q418" s="5"/>
+      <c r="R418" s="5"/>
+      <c r="S418" s="5"/>
+      <c r="T418" s="5"/>
+      <c r="U418" s="5"/>
+      <c r="V418" s="5"/>
+      <c r="W418" s="5"/>
+      <c r="X418" s="5"/>
     </row>
     <row r="419" spans="1:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="A419" s="4">
-        <v>509</v>
-      </c>
-      <c r="B419" t="s">
-        <v>441</v>
-      </c>
-      <c r="C419" s="5">
-        <v>0</v>
-      </c>
-      <c r="D419" s="5">
-        <v>0</v>
-      </c>
-      <c r="E419" s="5">
-        <v>0</v>
-      </c>
-      <c r="F419" s="5">
-        <v>0</v>
-      </c>
-      <c r="G419" s="5">
-        <v>0</v>
-      </c>
-      <c r="H419" s="5">
-        <v>0</v>
-      </c>
-      <c r="I419" s="5">
-        <v>0</v>
-      </c>
-      <c r="J419" s="5">
-        <v>0</v>
-      </c>
-      <c r="K419" s="5">
-        <v>0</v>
-      </c>
-      <c r="L419" s="5">
-        <v>0</v>
-      </c>
-      <c r="M419" s="5">
-        <v>0</v>
-      </c>
-      <c r="N419" s="5">
-        <v>0</v>
-      </c>
-      <c r="O419" s="5">
-        <v>0</v>
-      </c>
-      <c r="P419" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q419" s="5">
-        <v>0</v>
-      </c>
-      <c r="R419" s="5">
-        <v>0</v>
-      </c>
-      <c r="S419" s="5">
-        <v>0</v>
-      </c>
-      <c r="T419" s="5">
-        <v>0</v>
-      </c>
-      <c r="U419" s="5">
-        <v>0</v>
-      </c>
-      <c r="V419" s="5">
-        <v>0</v>
-      </c>
-      <c r="W419" s="5">
-        <v>0</v>
-      </c>
-      <c r="X419" s="5">
-        <v>0</v>
-      </c>
+      <c r="C419" s="5"/>
+      <c r="D419" s="5"/>
+      <c r="E419" s="5"/>
+      <c r="F419" s="5"/>
+      <c r="G419" s="5"/>
+      <c r="H419" s="5"/>
+      <c r="I419" s="5"/>
+      <c r="J419" s="5"/>
+      <c r="K419" s="5"/>
+      <c r="L419" s="5"/>
+      <c r="M419" s="5"/>
+      <c r="N419" s="5"/>
+      <c r="O419" s="5"/>
+      <c r="P419" s="5"/>
+      <c r="Q419" s="5"/>
+      <c r="R419" s="5"/>
+      <c r="S419" s="5"/>
+      <c r="T419" s="5"/>
+      <c r="U419" s="5"/>
+      <c r="V419" s="5"/>
+      <c r="W419" s="5"/>
+      <c r="X419" s="5"/>
     </row>
     <row r="420" spans="1:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="A420" s="4">
-        <v>510</v>
-      </c>
-      <c r="B420" t="s">
-        <v>442</v>
-      </c>
-      <c r="C420" s="5">
-        <v>0</v>
-      </c>
-      <c r="D420" s="5">
-        <v>0</v>
-      </c>
-      <c r="E420" s="5">
-        <v>0</v>
-      </c>
-      <c r="F420" s="5">
-        <v>0</v>
-      </c>
-      <c r="G420" s="5">
-        <v>0</v>
-      </c>
-      <c r="H420" s="5">
-        <v>0</v>
-      </c>
-      <c r="I420" s="5">
-        <v>0</v>
-      </c>
-      <c r="J420" s="5">
-        <v>0</v>
-      </c>
-      <c r="K420" s="5">
-        <v>0</v>
-      </c>
-      <c r="L420" s="5">
-        <v>0</v>
-      </c>
-      <c r="M420" s="5">
-        <v>0</v>
-      </c>
-      <c r="N420" s="5">
-        <v>0</v>
-      </c>
-      <c r="O420" s="5">
-        <v>0</v>
-      </c>
-      <c r="P420" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q420" s="5">
-        <v>0</v>
-      </c>
-      <c r="R420" s="5">
-        <v>0</v>
-      </c>
-      <c r="S420" s="5">
-        <v>0</v>
-      </c>
-      <c r="T420" s="5">
-        <v>0</v>
-      </c>
-      <c r="U420" s="5">
-        <v>0</v>
-      </c>
-      <c r="V420" s="5">
-        <v>0</v>
-      </c>
-      <c r="W420" s="5">
-        <v>0</v>
-      </c>
-      <c r="X420" s="5">
-        <v>0</v>
-      </c>
+      <c r="C420" s="5"/>
+      <c r="D420" s="5"/>
+      <c r="E420" s="5"/>
+      <c r="F420" s="5"/>
+      <c r="G420" s="5"/>
+      <c r="H420" s="5"/>
+      <c r="I420" s="5"/>
+      <c r="J420" s="5"/>
+      <c r="K420" s="5"/>
+      <c r="L420" s="5"/>
+      <c r="M420" s="5"/>
+      <c r="N420" s="5"/>
+      <c r="O420" s="5"/>
+      <c r="P420" s="5"/>
+      <c r="Q420" s="5"/>
+      <c r="R420" s="5"/>
+      <c r="S420" s="5"/>
+      <c r="T420" s="5"/>
+      <c r="U420" s="5"/>
+      <c r="V420" s="5"/>
+      <c r="W420" s="5"/>
+      <c r="X420" s="5"/>
     </row>
     <row r="421" spans="1:24" ht="13" x14ac:dyDescent="0.15">
       <c r="C421" s="5"/>
@@ -47059,136 +46876,26 @@
       <c r="W1010" s="5"/>
       <c r="X1010" s="5"/>
     </row>
-    <row r="1011" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1011" s="5"/>
-      <c r="D1011" s="5"/>
-      <c r="E1011" s="5"/>
-      <c r="F1011" s="5"/>
-      <c r="G1011" s="5"/>
-      <c r="H1011" s="5"/>
-      <c r="I1011" s="5"/>
-      <c r="J1011" s="5"/>
-      <c r="K1011" s="5"/>
-      <c r="L1011" s="5"/>
-      <c r="M1011" s="5"/>
-      <c r="N1011" s="5"/>
-      <c r="O1011" s="5"/>
-      <c r="P1011" s="5"/>
-      <c r="Q1011" s="5"/>
-      <c r="R1011" s="5"/>
-      <c r="S1011" s="5"/>
-      <c r="T1011" s="5"/>
-      <c r="U1011" s="5"/>
-      <c r="V1011" s="5"/>
-      <c r="W1011" s="5"/>
-      <c r="X1011" s="5"/>
-    </row>
-    <row r="1012" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1012" s="5"/>
-      <c r="D1012" s="5"/>
-      <c r="E1012" s="5"/>
-      <c r="F1012" s="5"/>
-      <c r="G1012" s="5"/>
-      <c r="H1012" s="5"/>
-      <c r="I1012" s="5"/>
-      <c r="J1012" s="5"/>
-      <c r="K1012" s="5"/>
-      <c r="L1012" s="5"/>
-      <c r="M1012" s="5"/>
-      <c r="N1012" s="5"/>
-      <c r="O1012" s="5"/>
-      <c r="P1012" s="5"/>
-      <c r="Q1012" s="5"/>
-      <c r="R1012" s="5"/>
-      <c r="S1012" s="5"/>
-      <c r="T1012" s="5"/>
-      <c r="U1012" s="5"/>
-      <c r="V1012" s="5"/>
-      <c r="W1012" s="5"/>
-      <c r="X1012" s="5"/>
-    </row>
-    <row r="1013" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1013" s="5"/>
-      <c r="D1013" s="5"/>
-      <c r="E1013" s="5"/>
-      <c r="F1013" s="5"/>
-      <c r="G1013" s="5"/>
-      <c r="H1013" s="5"/>
-      <c r="I1013" s="5"/>
-      <c r="J1013" s="5"/>
-      <c r="K1013" s="5"/>
-      <c r="L1013" s="5"/>
-      <c r="M1013" s="5"/>
-      <c r="N1013" s="5"/>
-      <c r="O1013" s="5"/>
-      <c r="P1013" s="5"/>
-      <c r="Q1013" s="5"/>
-      <c r="R1013" s="5"/>
-      <c r="S1013" s="5"/>
-      <c r="T1013" s="5"/>
-      <c r="U1013" s="5"/>
-      <c r="V1013" s="5"/>
-      <c r="W1013" s="5"/>
-      <c r="X1013" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C417 D2:W14 D16:W16 D15:X15 D17:X17 D18:W246 D248:W417 C418:W418">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+  <conditionalFormatting sqref="C2:C417 D248:W417">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C417 D2:W14 D16:W16 D15:X15 D17:X17 D18:W246 D248:W417 C418:W418">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+  <conditionalFormatting sqref="X248:X417 D2:X246">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C417 D2:W14 D16:W16 D15:X15 D17:X17 D18:W246 D248:W417 C418:W418">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X14 X16 X18:X246 X248:X420">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X14 X16 X18:X246 X248:X420">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X14 X16 X18:X246 X248:X420">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C419:W419">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C419:W419">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C419:W419">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C420:W420">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C420:W420">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C420:W420">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>